<commit_message>
starting augmentation process (for actor)
</commit_message>
<xml_diff>
--- a/GPT_labeling/prompt-comparison-results.xlsx
+++ b/GPT_labeling/prompt-comparison-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annalieb/Documents/Thesis/Senior-Thesis/GPT_labeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4284060D-77ED-3B42-8462-C53F50ED7694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1870CAF1-768B-0749-9E51-6E4D51C52053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="740" windowWidth="23600" windowHeight="17240" xr2:uid="{92BB175C-204B-7844-8714-001F5ACED15C}"/>
+    <workbookView xWindow="1540" yWindow="740" windowWidth="23600" windowHeight="17240" activeTab="1" xr2:uid="{92BB175C-204B-7844-8714-001F5ACED15C}"/>
   </bookViews>
   <sheets>
     <sheet name="actor" sheetId="1" r:id="rId1"/>
@@ -2656,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC5BDC4-8E72-AD46-BB16-EE1C2B121936}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2728,8 +2728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6A9FF9-DD24-9948-BDE4-FAC7106C6C51}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Finish time series modeling
</commit_message>
<xml_diff>
--- a/GPT_labeling/prompt-comparison-results.xlsx
+++ b/GPT_labeling/prompt-comparison-results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annalieb/Documents/Thesis/Senior-Thesis/GPT_labeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7532F66-9569-DF44-AEB9-A4071E4CCC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1907BE3E-39D7-D349-8F36-118C04842CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="23600" windowHeight="17240" xr2:uid="{92BB175C-204B-7844-8714-001F5ACED15C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="23600" windowHeight="17240" activeTab="1" xr2:uid="{92BB175C-204B-7844-8714-001F5ACED15C}"/>
   </bookViews>
   <sheets>
     <sheet name="actor" sheetId="1" r:id="rId1"/>
@@ -37,16 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>augmentation</t>
-  </si>
-  <si>
-    <t>baseline</t>
-  </si>
-  <si>
-    <t>intuitive</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>0 examples</t>
   </si>
@@ -135,69 +126,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>GPT-4 Performance for Actor</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1167,67 +1096,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>GPT-4</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Performance for Stance</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1243,7 +1112,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>baseline</c:v>
+                  <c:v>Prompt includes examples only (no definition)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1314,7 +1183,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>intuitive</c:v>
+                  <c:v>Prompt includes examples and definitions</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3744,7 +3613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC5BDC4-8E72-AD46-BB16-EE1C2B121936}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+    <sheetView zoomScale="106" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3755,24 +3624,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0.68385111361628204</v>
@@ -3786,7 +3655,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.83389941918805999</v>
@@ -3809,34 +3678,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6A9FF9-DD24-9948-BDE4-FAC7106C6C51}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0.70143136200594802</v>
@@ -3850,7 +3719,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0.76816505328432605</v>
@@ -3865,11 +3734,6 @@
         <v>0.75407622344659098</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>